<commit_message>
Fix bug related to selection of successful experiments in batch2
</commit_message>
<xml_diff>
--- a/suggested_experiments/experiments_batch2.xlsx
+++ b/suggested_experiments/experiments_batch2.xlsx
@@ -484,7 +484,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F2" t="n">
         <v>130</v>
@@ -501,25 +501,25 @@
         <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>90</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
         <v>1.5</v>
       </c>
       <c r="F3" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G3" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
@@ -530,22 +530,22 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>80</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F4" t="n">
         <v>125</v>
       </c>
       <c r="G4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H4" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
@@ -553,25 +553,25 @@
         <v>44</v>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>55.00000000000001</v>
+        <v>85.00000000000001</v>
       </c>
       <c r="D5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
         <v>1.5</v>
       </c>
       <c r="F5" t="n">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G5" t="n">
         <v>20</v>
       </c>
       <c r="H5" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6">
@@ -588,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="E6" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F6" t="n">
         <v>130</v>
@@ -597,7 +597,7 @@
         <v>20</v>
       </c>
       <c r="H6" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7">
@@ -611,19 +611,19 @@
         <v>85.00000000000001</v>
       </c>
       <c r="D7" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E7" t="n">
         <v>1.5</v>
       </c>
       <c r="F7" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G7" t="n">
         <v>20</v>
       </c>
       <c r="H7" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -640,7 +640,7 @@
         <v>10</v>
       </c>
       <c r="E8" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F8" t="n">
         <v>125</v>
@@ -660,22 +660,22 @@
         <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>90</v>
+        <v>85.00000000000001</v>
       </c>
       <c r="D9" t="n">
         <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F9" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G9" t="n">
         <v>20</v>
       </c>
       <c r="H9" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
@@ -686,13 +686,13 @@
         <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>85.00000000000001</v>
+        <v>90</v>
       </c>
       <c r="D10" t="n">
         <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F10" t="n">
         <v>130</v>
@@ -701,7 +701,7 @@
         <v>20</v>
       </c>
       <c r="H10" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -712,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D11" t="n">
         <v>10</v>
@@ -721,13 +721,13 @@
         <v>1.5</v>
       </c>
       <c r="F11" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G11" t="n">
         <v>20</v>
       </c>
       <c r="H11" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -741,10 +741,10 @@
         <v>85.00000000000001</v>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E12" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="F12" t="n">
         <v>125</v>
@@ -753,7 +753,7 @@
         <v>20</v>
       </c>
       <c r="H12" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -761,13 +761,13 @@
         <v>52</v>
       </c>
       <c r="B13" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>70</v>
+        <v>85.00000000000001</v>
       </c>
       <c r="D13" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E13" t="n">
         <v>1.5</v>
@@ -776,10 +776,10 @@
         <v>125</v>
       </c>
       <c r="G13" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H13" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
@@ -799,13 +799,13 @@
         <v>1.4</v>
       </c>
       <c r="F14" t="n">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G14" t="n">
         <v>20</v>
       </c>
       <c r="H14" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15">
@@ -816,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D15" t="n">
         <v>10</v>
@@ -825,13 +825,13 @@
         <v>1.5</v>
       </c>
       <c r="F15" t="n">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="G15" t="n">
         <v>20</v>
       </c>
       <c r="H15" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -842,22 +842,22 @@
         <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>55.00000000000001</v>
+        <v>90</v>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E16" t="n">
         <v>1.4</v>
       </c>
       <c r="F16" t="n">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G16" t="n">
         <v>20</v>
       </c>
       <c r="H16" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -868,13 +868,13 @@
         <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D17" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F17" t="n">
         <v>125</v>
@@ -883,7 +883,7 @@
         <v>20</v>
       </c>
       <c r="H17" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18">
@@ -894,7 +894,7 @@
         <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>90</v>
+        <v>85.00000000000001</v>
       </c>
       <c r="D18" t="n">
         <v>10</v>
@@ -909,7 +909,7 @@
         <v>20</v>
       </c>
       <c r="H18" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19">
@@ -920,16 +920,16 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>90</v>
+        <v>85.00000000000001</v>
       </c>
       <c r="D19" t="n">
         <v>15</v>
       </c>
       <c r="E19" t="n">
-        <v>1.4</v>
+        <v>1.5</v>
       </c>
       <c r="F19" t="n">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G19" t="n">
         <v>20</v>
@@ -946,22 +946,22 @@
         <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>90</v>
+        <v>85.00000000000001</v>
       </c>
       <c r="D20" t="n">
         <v>10</v>
       </c>
       <c r="E20" t="n">
-        <v>1.4</v>
+        <v>1.6</v>
       </c>
       <c r="F20" t="n">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G20" t="n">
         <v>20</v>
       </c>
       <c r="H20" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21">
@@ -972,16 +972,16 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>85.00000000000001</v>
+        <v>80</v>
       </c>
       <c r="D21" t="n">
         <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>1.6</v>
+        <v>1.4</v>
       </c>
       <c r="F21" t="n">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="G21" t="n">
         <v>20</v>

</xml_diff>